<commit_message>
modification liste de course
</commit_message>
<xml_diff>
--- a/feuille de course.xlsx
+++ b/feuille de course.xlsx
@@ -11,22 +11,60 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>LB1930M</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Composant</t>
+  </si>
+  <si>
+    <t>Référence</t>
+  </si>
+  <si>
+    <t>Pont en H</t>
+  </si>
+  <si>
+    <t>Lien</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>LB1930MC-AH</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/on-semiconductor/lb1930mc-ah/motor-driver-dc-brush-1a-soic/dp/2458869</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Prix unitaire</t>
+  </si>
+  <si>
+    <t>Prix total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -42,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -50,12 +88,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,19 +529,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1.46</v>
+      </c>
+      <c r="G3" s="11">
+        <f>F3*C3</f>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G15" si="0">F4*C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="10">
+        <f>SUM(G3:G15)</f>
+        <v>2.92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ajout 5 tio 3.3 i²c liste course
</commit_message>
<xml_diff>
--- a/feuille de course.xlsx
+++ b/feuille de course.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Composant</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Prix total</t>
+  </si>
+  <si>
+    <t>PCA9306D</t>
+  </si>
+  <si>
+    <t>5 to 3,3 bidir i²c</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/nxp/pca9306d/ic-i2c-smbus-volt-trans-double/dp/2212070?ost=2212070&amp;mckv=sS7zBkBKq_dc%7Cpcrid%7C79324297994%7Ckword%7Cpca9306d%7Cmatch%7Cp%7Cplid%7C&amp;CMP=KNC-GFR-FFR-GEN-SKU-MDC&amp;gclid=CIzq7vvXm8gCFRITGwodfYMC8w</t>
   </si>
 </sst>
 </file>
@@ -55,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +80,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,10 +224,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -228,8 +246,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,7 +552,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,14 +607,24 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.76400000000000001</v>
+      </c>
       <c r="G4" s="11">
         <f t="shared" ref="G4:G15" si="0">F4*C4</f>
-        <v>0</v>
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -725,12 +755,15 @@
       <c r="F17" s="4"/>
       <c r="G17" s="10">
         <f>SUM(G3:G15)</f>
-        <v>2.92</v>
+        <v>3.6840000000000002</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update feuille de course
</commit_message>
<xml_diff>
--- a/feuille de course.xlsx
+++ b/feuille de course.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Composant</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>http://fr.farnell.com/nxp/pca9306d/ic-i2c-smbus-volt-trans-double/dp/2212070?ost=2212070&amp;mckv=sS7zBkBKq_dc%7Cpcrid%7C79324297994%7Ckword%7Cpca9306d%7Cmatch%7Cp%7Cplid%7C&amp;CMP=KNC-GFR-FFR-GEN-SKU-MDC&amp;gclid=CIzq7vvXm8gCFRITGwodfYMC8w</t>
+  </si>
+  <si>
+    <t>MAX1237EUA+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN I²C </t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/can-a-usage-general/7327670/?searchTerm=MAX1237EUA%2B&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D6672266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D313326736E3D592673743D4D414E5F504152545F4E554D4245522677633D424F5448267573743D4D4158313233374555412B26&amp;sra=p</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -247,6 +256,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -628,14 +638,24 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11"/>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="11">
+        <v>9.48</v>
+      </c>
       <c r="G5" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -755,12 +775,13 @@
       <c r="F17" s="4"/>
       <c r="G17" s="10">
         <f>SUM(G3:G15)</f>
-        <v>3.6840000000000002</v>
+        <v>13.164000000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" r:id="rId2"/>

</xml_diff>